<commit_message>
planilla de turno vercion tres
</commit_message>
<xml_diff>
--- a/Planillas/Planillas xls/planilla varios primera version.xlsx
+++ b/Planillas/Planillas xls/planilla varios primera version.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$B$3:$H$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$B$2:$H$43</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>GTX 20W-50 X 4L</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>LIQUI MOLI DIESEL</t>
+  </si>
+  <si>
+    <t>GTX 15W-40 X 4L</t>
   </si>
 </sst>
 </file>
@@ -441,6 +444,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -449,15 +461,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -764,7 +767,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -777,8 +780,8 @@
   </sheetPr>
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A34" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -787,7 +790,7 @@
     <col min="3" max="8" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -800,50 +803,52 @@
     </row>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="B2" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="32.1" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16"/>
-    </row>
-    <row r="4" spans="1:9" ht="24.95" customHeight="1" thickBot="1">
+      <c r="B3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="24.95" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="B4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1">
       <c r="A5" s="1"/>
@@ -1295,22 +1300,22 @@
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
       <c r="E42" s="13"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
       <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:9" ht="30" customHeight="1" thickBot="1">
-      <c r="A43" s="23"/>
-      <c r="B43" s="17" t="s">
+      <c r="A43" s="20"/>
+      <c r="B43" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="20"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="22"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="19"/>
     </row>
     <row r="44" spans="1:9" ht="30" customHeight="1">
       <c r="A44" s="1"/>
@@ -1328,7 +1333,7 @@
     <row r="49" ht="30" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="portrait" verticalDpi="1200" r:id="rId1"/>

</xml_diff>